<commit_message>
Atualização Documentação controle de tabelas
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="27" activeTab="33"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sequência Execução" sheetId="35" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10510" uniqueCount="2828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10525" uniqueCount="2832">
   <si>
     <t>Processo de Carga LN</t>
   </si>
@@ -8531,6 +8531,18 @@
   </si>
   <si>
     <t>N:\Migracao\Despesas_LN\Despesas_LN\stg_despesas_ln.dtsx</t>
+  </si>
+  <si>
+    <t>(DFT) WMS - Romaneio</t>
+  </si>
+  <si>
+    <t>dbo.stg_wms_romaneio</t>
+  </si>
+  <si>
+    <t>(DFT) Romaneio</t>
+  </si>
+  <si>
+    <t>ln.ods_wms_romaneio</t>
   </si>
 </sst>
 </file>
@@ -8970,30 +8982,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9020,6 +9008,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9338,7 +9350,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="65" t="s">
         <v>279</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -9349,7 +9361,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1">
-      <c r="A3" s="54"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="25" t="s">
         <v>997</v>
       </c>
@@ -9358,7 +9370,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
-      <c r="A4" s="54"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="25" t="s">
         <v>1203</v>
       </c>
@@ -9367,7 +9379,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1">
-      <c r="A5" s="54"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="25" t="s">
         <v>1362</v>
       </c>
@@ -9376,7 +9388,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1">
-      <c r="A6" s="54"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="25" t="s">
         <v>1553</v>
       </c>
@@ -9385,7 +9397,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1">
-      <c r="A7" s="54"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="25" t="s">
         <v>2214</v>
       </c>
@@ -9394,7 +9406,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1">
-      <c r="A8" s="54"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="25" t="s">
         <v>1957</v>
       </c>
@@ -9403,7 +9415,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
-      <c r="A9" s="54"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="25" t="s">
         <v>2227</v>
       </c>
@@ -9412,7 +9424,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
-      <c r="A10" s="54"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="25" t="s">
         <v>801</v>
       </c>
@@ -9421,7 +9433,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
-      <c r="A11" s="55"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="25" t="s">
         <v>1479</v>
       </c>
@@ -9430,7 +9442,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="65" t="s">
         <v>285</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -9441,7 +9453,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1">
-      <c r="A13" s="54"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="25" t="s">
         <v>995</v>
       </c>
@@ -9450,7 +9462,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1">
-      <c r="A14" s="54"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="25" t="s">
         <v>997</v>
       </c>
@@ -9459,7 +9471,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">
-      <c r="A15" s="54"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="25" t="s">
         <v>1320</v>
       </c>
@@ -9468,7 +9480,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1">
-      <c r="A16" s="54"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="25" t="s">
         <v>1362</v>
       </c>
@@ -9477,7 +9489,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
-      <c r="A17" s="54"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="25" t="s">
         <v>1479</v>
       </c>
@@ -9486,7 +9498,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
-      <c r="A18" s="54"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="25" t="s">
         <v>1567</v>
       </c>
@@ -9495,7 +9507,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
-      <c r="A19" s="54"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="25" t="s">
         <v>1693</v>
       </c>
@@ -9504,7 +9516,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
-      <c r="A20" s="54"/>
+      <c r="A20" s="66"/>
       <c r="B20" s="25" t="s">
         <v>2227</v>
       </c>
@@ -9513,7 +9525,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1">
-      <c r="A21" s="55"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="52" t="s">
         <v>701</v>
       </c>
@@ -9522,7 +9534,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="65" t="s">
         <v>733</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -9533,7 +9545,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
-      <c r="A23" s="54"/>
+      <c r="A23" s="66"/>
       <c r="B23" s="25" t="s">
         <v>888</v>
       </c>
@@ -9542,7 +9554,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
-      <c r="A24" s="54"/>
+      <c r="A24" s="66"/>
       <c r="B24" s="25" t="s">
         <v>995</v>
       </c>
@@ -9551,7 +9563,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1">
-      <c r="A25" s="54"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="25" t="s">
         <v>1567</v>
       </c>
@@ -9560,7 +9572,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
-      <c r="A26" s="54"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="25" t="s">
         <v>1693</v>
       </c>
@@ -9569,7 +9581,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
-      <c r="A27" s="54"/>
+      <c r="A27" s="66"/>
       <c r="B27" s="25" t="s">
         <v>1957</v>
       </c>
@@ -9578,7 +9590,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1">
-      <c r="A28" s="54"/>
+      <c r="A28" s="66"/>
       <c r="B28" s="25" t="s">
         <v>2227</v>
       </c>
@@ -9587,7 +9599,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1">
-      <c r="A29" s="54"/>
+      <c r="A29" s="66"/>
       <c r="B29" s="25" t="s">
         <v>2343</v>
       </c>
@@ -9596,7 +9608,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1">
-      <c r="A30" s="55"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="25" t="s">
         <v>801</v>
       </c>
@@ -9616,7 +9628,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="65" t="s">
         <v>1362</v>
       </c>
       <c r="B32" s="25" t="s">
@@ -9627,7 +9639,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1">
-      <c r="A33" s="55"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="25" t="s">
         <v>1986</v>
       </c>
@@ -9636,7 +9648,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="65" t="s">
         <v>1479</v>
       </c>
       <c r="B34" s="25" t="s">
@@ -9647,7 +9659,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1">
-      <c r="A35" s="54"/>
+      <c r="A35" s="66"/>
       <c r="B35" s="25" t="s">
         <v>1535</v>
       </c>
@@ -9656,7 +9668,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1">
-      <c r="A36" s="54"/>
+      <c r="A36" s="66"/>
       <c r="B36" s="25" t="s">
         <v>1986</v>
       </c>
@@ -9665,7 +9677,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1">
-      <c r="A37" s="55"/>
+      <c r="A37" s="67"/>
       <c r="B37" s="25" t="s">
         <v>2016</v>
       </c>
@@ -9707,7 +9719,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="65" t="s">
         <v>2473</v>
       </c>
       <c r="B41" s="25" t="s">
@@ -9718,7 +9730,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1">
-      <c r="A42" s="54"/>
+      <c r="A42" s="66"/>
       <c r="B42" s="25" t="s">
         <v>1986</v>
       </c>
@@ -9727,7 +9739,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1">
-      <c r="A43" s="54"/>
+      <c r="A43" s="66"/>
       <c r="B43" s="25" t="s">
         <v>2177</v>
       </c>
@@ -9736,7 +9748,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1">
-      <c r="A44" s="54"/>
+      <c r="A44" s="66"/>
       <c r="B44" s="25" t="s">
         <v>2099</v>
       </c>
@@ -9745,7 +9757,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1">
-      <c r="A45" s="55"/>
+      <c r="A45" s="67"/>
       <c r="B45" s="25" t="s">
         <v>1931</v>
       </c>
@@ -9765,7 +9777,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="65" t="s">
         <v>2016</v>
       </c>
       <c r="B47" s="25" t="s">
@@ -9776,7 +9788,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1">
-      <c r="A48" s="55"/>
+      <c r="A48" s="67"/>
       <c r="B48" s="25" t="s">
         <v>1418</v>
       </c>
@@ -11817,39 +11829,39 @@
     <col min="7" max="7" width="54.140625" style="44" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="44" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45.5703125" style="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.85546875" style="71" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.85546875" style="63" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="68" customFormat="1" ht="27.95" customHeight="1">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:10" s="60" customFormat="1" ht="27.95" customHeight="1">
+      <c r="A1" s="57" t="s">
         <v>705</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="58" t="s">
         <v>706</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="58" t="s">
         <v>710</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="58" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="58" t="s">
         <v>708</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="58" t="s">
         <v>707</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="58" t="s">
         <v>709</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="59" t="s">
         <v>714</v>
       </c>
     </row>
@@ -14780,28 +14792,28 @@
       <c r="J97" s="50"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="72" t="s">
+      <c r="A98" s="64" t="s">
         <v>1119</v>
       </c>
-      <c r="B98" s="62"/>
-      <c r="C98" s="62"/>
-      <c r="D98" s="62"/>
-      <c r="E98" s="62" t="s">
+      <c r="B98" s="54"/>
+      <c r="C98" s="54"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="54" t="s">
         <v>2814</v>
       </c>
-      <c r="F98" s="62" t="s">
+      <c r="F98" s="54" t="s">
         <v>2815</v>
       </c>
-      <c r="G98" s="62" t="s">
+      <c r="G98" s="54" t="s">
         <v>2816</v>
       </c>
-      <c r="H98" s="62" t="s">
+      <c r="H98" s="54" t="s">
         <v>398</v>
       </c>
-      <c r="I98" s="62" t="s">
+      <c r="I98" s="54" t="s">
         <v>2817</v>
       </c>
-      <c r="J98" s="63" t="s">
+      <c r="J98" s="55" t="s">
         <v>2818</v>
       </c>
     </row>
@@ -15391,7 +15403,7 @@
     </row>
     <row r="120" spans="1:10" ht="12.75">
       <c r="A120" s="45"/>
-      <c r="B120" s="69"/>
+      <c r="B120" s="61"/>
       <c r="C120" s="46"/>
       <c r="D120" s="46"/>
       <c r="E120" s="46"/>
@@ -15399,7 +15411,7 @@
       <c r="G120" s="46"/>
       <c r="H120" s="46"/>
       <c r="I120" s="46"/>
-      <c r="J120" s="70"/>
+      <c r="J120" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -19612,7 +19624,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="68" t="s">
         <v>279</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -19627,7 +19639,7 @@
       <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="56"/>
+      <c r="A3" s="68"/>
       <c r="B3" s="25" t="s">
         <v>282</v>
       </c>
@@ -19640,7 +19652,7 @@
       <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="56"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="25" t="s">
         <v>283</v>
       </c>
@@ -19653,7 +19665,7 @@
       <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="68" t="s">
         <v>285</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -19668,7 +19680,7 @@
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="56"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="31" t="s">
         <v>377</v>
       </c>
@@ -19681,7 +19693,7 @@
       <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="56"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="31" t="s">
         <v>432</v>
       </c>
@@ -19694,7 +19706,7 @@
       <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="56"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="25" t="s">
         <v>442</v>
       </c>
@@ -19722,7 +19734,7 @@
       <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="68" t="s">
         <v>733</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -19737,7 +19749,7 @@
       <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="56"/>
+      <c r="A11" s="68"/>
       <c r="B11" s="25" t="s">
         <v>749</v>
       </c>
@@ -19750,7 +19762,7 @@
       <c r="E11" s="26"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="56"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="25" t="s">
         <v>738</v>
       </c>
@@ -19763,7 +19775,7 @@
       <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="25" t="s">
         <v>756</v>
       </c>
@@ -19776,7 +19788,7 @@
       <c r="E13" s="26"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="56"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="25" t="s">
         <v>762</v>
       </c>
@@ -19789,7 +19801,7 @@
       <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="56"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="25" t="s">
         <v>763</v>
       </c>
@@ -19802,7 +19814,7 @@
       <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="56"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="25" t="s">
         <v>775</v>
       </c>
@@ -19815,7 +19827,7 @@
       <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
-      <c r="A17" s="56"/>
+      <c r="A17" s="68"/>
       <c r="B17" s="25" t="s">
         <v>776</v>
       </c>
@@ -19828,7 +19840,7 @@
       <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="56"/>
+      <c r="A18" s="68"/>
       <c r="B18" s="25" t="s">
         <v>797</v>
       </c>
@@ -19856,7 +19868,7 @@
       <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="71" t="s">
         <v>2640</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -19871,7 +19883,7 @@
       <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="60"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="25" t="s">
         <v>2644</v>
       </c>
@@ -19899,7 +19911,7 @@
       <c r="E22" s="26"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="68" t="s">
         <v>888</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -19916,7 +19928,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
-      <c r="A24" s="56"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="25" t="s">
         <v>890</v>
       </c>
@@ -19929,7 +19941,7 @@
       <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
-      <c r="A25" s="56"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="31" t="s">
         <v>891</v>
       </c>
@@ -19942,7 +19954,7 @@
       <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
-      <c r="A26" s="56"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="25" t="s">
         <v>892</v>
       </c>
@@ -19970,7 +19982,7 @@
       <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="68" t="s">
         <v>997</v>
       </c>
       <c r="B28" s="31" t="s">
@@ -19985,7 +19997,7 @@
       <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="56"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="31" t="s">
         <v>147</v>
       </c>
@@ -19998,7 +20010,7 @@
       <c r="E29" s="26"/>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
-      <c r="A30" s="56"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="31" t="s">
         <v>998</v>
       </c>
@@ -20011,7 +20023,7 @@
       <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
-      <c r="A31" s="56"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="31" t="s">
         <v>999</v>
       </c>
@@ -20026,7 +20038,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="68" t="s">
         <v>1203</v>
       </c>
       <c r="B32" s="25" t="s">
@@ -20041,7 +20053,7 @@
       <c r="E32" s="26"/>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1">
-      <c r="A33" s="56"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="25" t="s">
         <v>1205</v>
       </c>
@@ -20054,7 +20066,7 @@
       <c r="E33" s="26"/>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1">
-      <c r="A34" s="56"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="25" t="s">
         <v>1206</v>
       </c>
@@ -20067,7 +20079,7 @@
       <c r="E34" s="26"/>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1">
-      <c r="A35" s="56"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="25" t="s">
         <v>1207</v>
       </c>
@@ -20080,7 +20092,7 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
-      <c r="A36" s="56"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="25" t="s">
         <v>1208</v>
       </c>
@@ -20093,7 +20105,7 @@
       <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="68" t="s">
         <v>1320</v>
       </c>
       <c r="B37" s="25" t="s">
@@ -20108,7 +20120,7 @@
       <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
-      <c r="A38" s="56"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="25" t="s">
         <v>1322</v>
       </c>
@@ -20123,7 +20135,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="68" t="s">
         <v>1362</v>
       </c>
       <c r="B39" s="25" t="s">
@@ -20138,7 +20150,7 @@
       <c r="E39" s="26"/>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
-      <c r="A40" s="56"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="25" t="s">
         <v>1364</v>
       </c>
@@ -20166,7 +20178,7 @@
       <c r="E41" s="26"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="68" t="s">
         <v>1479</v>
       </c>
       <c r="B42" s="25" t="s">
@@ -20181,7 +20193,7 @@
       <c r="E42" s="26"/>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1">
-      <c r="A43" s="56"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="25" t="s">
         <v>1481</v>
       </c>
@@ -20224,7 +20236,7 @@
       <c r="E45" s="26"/>
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="68" t="s">
         <v>1567</v>
       </c>
       <c r="B46" s="25" t="s">
@@ -20239,7 +20251,7 @@
       <c r="E46" s="26"/>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1">
-      <c r="A47" s="56"/>
+      <c r="A47" s="68"/>
       <c r="B47" s="25" t="s">
         <v>1569</v>
       </c>
@@ -20314,7 +20326,7 @@
       <c r="E51" s="26"/>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="68" t="s">
         <v>1986</v>
       </c>
       <c r="B52" s="25" t="s">
@@ -20329,7 +20341,7 @@
       <c r="E52" s="26"/>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
-      <c r="A53" s="56"/>
+      <c r="A53" s="68"/>
       <c r="B53" s="25" t="s">
         <v>1988</v>
       </c>
@@ -20417,7 +20429,7 @@
       <c r="E58" s="26"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1">
-      <c r="A59" s="56" t="s">
+      <c r="A59" s="68" t="s">
         <v>2227</v>
       </c>
       <c r="B59" s="25" t="s">
@@ -20432,7 +20444,7 @@
       <c r="E59" s="26"/>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1">
-      <c r="A60" s="56"/>
+      <c r="A60" s="68"/>
       <c r="B60" s="25" t="s">
         <v>2231</v>
       </c>
@@ -20445,7 +20457,7 @@
       <c r="E60" s="26"/>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1">
-      <c r="A61" s="56"/>
+      <c r="A61" s="68"/>
       <c r="B61" s="25" t="s">
         <v>2234</v>
       </c>
@@ -20458,7 +20470,7 @@
       <c r="E61" s="26"/>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="69" t="s">
         <v>2343</v>
       </c>
       <c r="B62" s="25" t="s">
@@ -20473,7 +20485,7 @@
       <c r="E62" s="26"/>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1">
-      <c r="A63" s="57"/>
+      <c r="A63" s="69"/>
       <c r="B63" s="25" t="s">
         <v>2347</v>
       </c>
@@ -20486,7 +20498,7 @@
       <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1">
-      <c r="A64" s="57"/>
+      <c r="A64" s="69"/>
       <c r="B64" s="25" t="s">
         <v>2350</v>
       </c>
@@ -20501,7 +20513,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1">
-      <c r="A65" s="57"/>
+      <c r="A65" s="69"/>
       <c r="B65" s="25" t="s">
         <v>2353</v>
       </c>
@@ -20514,7 +20526,7 @@
       <c r="E65" s="26"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1">
-      <c r="A66" s="57"/>
+      <c r="A66" s="69"/>
       <c r="B66" s="25" t="s">
         <v>2356</v>
       </c>
@@ -20527,7 +20539,7 @@
       <c r="E66" s="26"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1">
-      <c r="A67" s="56" t="s">
+      <c r="A67" s="68" t="s">
         <v>2389</v>
       </c>
       <c r="B67" s="25" t="s">
@@ -20542,7 +20554,7 @@
       <c r="E67" s="26"/>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1">
-      <c r="A68" s="56"/>
+      <c r="A68" s="68"/>
       <c r="B68" s="25" t="s">
         <v>2391</v>
       </c>
@@ -20557,7 +20569,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1">
-      <c r="A69" s="56"/>
+      <c r="A69" s="68"/>
       <c r="B69" s="31" t="s">
         <v>2392</v>
       </c>
@@ -20570,7 +20582,7 @@
       <c r="E69" s="26"/>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1">
-      <c r="A70" s="56"/>
+      <c r="A70" s="68"/>
       <c r="B70" s="31" t="s">
         <v>2393</v>
       </c>
@@ -20585,7 +20597,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="58"/>
+      <c r="A71" s="70"/>
       <c r="B71" s="36" t="s">
         <v>2394</v>
       </c>
@@ -30251,11 +30263,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -32031,29 +32043,27 @@
         <v>281</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>122</v>
+        <v>2</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>125</v>
+        <v>2828</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J59" s="9" t="s">
-        <v>102</v>
-      </c>
+        <v>2829</v>
+      </c>
+      <c r="J59" s="9"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="5" t="s">
@@ -32075,13 +32085,13 @@
         <v>124</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J60" s="9" t="s">
         <v>102</v>
@@ -32098,24 +32108,26 @@
         <v>122</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="J61" s="9"/>
+        <v>128</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="5" t="s">
@@ -32137,13 +32149,13 @@
         <v>130</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J62" s="9"/>
     </row>
@@ -32167,13 +32179,13 @@
         <v>130</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J63" s="9"/>
     </row>
@@ -32197,13 +32209,13 @@
         <v>130</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J64" s="9"/>
     </row>
@@ -32227,13 +32239,13 @@
         <v>130</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H65" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J65" s="9"/>
     </row>
@@ -32257,13 +32269,13 @@
         <v>130</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J66" s="9"/>
     </row>
@@ -32287,13 +32299,13 @@
         <v>130</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J67" s="9"/>
     </row>
@@ -32317,13 +32329,13 @@
         <v>130</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J68" s="9"/>
     </row>
@@ -32338,22 +32350,22 @@
         <v>122</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J69" s="9"/>
     </row>
@@ -32377,13 +32389,13 @@
         <v>148</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J70" s="9"/>
     </row>
@@ -32407,13 +32419,13 @@
         <v>148</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J71" s="9"/>
     </row>
@@ -32437,13 +32449,13 @@
         <v>148</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J72" s="9"/>
     </row>
@@ -32467,13 +32479,13 @@
         <v>148</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H73" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J73" s="9"/>
     </row>
@@ -32497,13 +32509,13 @@
         <v>148</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J74" s="9"/>
     </row>
@@ -32518,22 +32530,22 @@
         <v>122</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J75" s="9"/>
     </row>
@@ -32548,22 +32560,22 @@
         <v>122</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J76" s="9"/>
     </row>
@@ -32587,13 +32599,13 @@
         <v>166</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J77" s="9"/>
     </row>
@@ -32617,13 +32629,13 @@
         <v>166</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J78" s="9"/>
     </row>
@@ -32647,13 +32659,13 @@
         <v>166</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J79" s="9"/>
     </row>
@@ -32668,22 +32680,22 @@
         <v>122</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J80" s="9"/>
     </row>
@@ -32698,22 +32710,22 @@
         <v>122</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I81" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J81" s="9"/>
     </row>
@@ -32737,13 +32749,13 @@
         <v>180</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J82" s="9"/>
     </row>
@@ -32758,22 +32770,22 @@
         <v>122</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I83" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J83" s="9"/>
     </row>
@@ -32788,22 +32800,22 @@
         <v>122</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J84" s="9"/>
     </row>
@@ -32827,13 +32839,13 @@
         <v>190</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H85" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J85" s="9"/>
     </row>
@@ -32857,13 +32869,13 @@
         <v>190</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J86" s="9"/>
     </row>
@@ -32887,13 +32899,13 @@
         <v>190</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J87" s="9"/>
     </row>
@@ -32917,13 +32929,13 @@
         <v>190</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J88" s="9"/>
     </row>
@@ -32938,22 +32950,22 @@
         <v>122</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I89" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J89" s="9"/>
     </row>
@@ -32977,13 +32989,13 @@
         <v>202</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H90" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J90" s="9"/>
     </row>
@@ -33007,13 +33019,13 @@
         <v>202</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H91" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J91" s="9"/>
     </row>
@@ -33043,7 +33055,7 @@
         <v>6</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>2615</v>
+        <v>208</v>
       </c>
       <c r="J92" s="9"/>
     </row>
@@ -33058,48 +33070,54 @@
         <v>122</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I93" s="6" t="s">
+        <v>2615</v>
+      </c>
+      <c r="J93" s="9"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I94" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="J93" s="9"/>
-    </row>
-    <row r="94" spans="1:10" s="44" customFormat="1">
-      <c r="A94" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B94" s="42" t="s">
-        <v>395</v>
-      </c>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
-      <c r="F94" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="G94" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="H94" s="42" t="s">
-        <v>215</v>
-      </c>
-      <c r="I94" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="J94" s="43"/>
+      <c r="J94" s="9"/>
     </row>
     <row r="95" spans="1:10" s="44" customFormat="1">
       <c r="A95" s="41" t="s">
@@ -33112,16 +33130,16 @@
       <c r="D95" s="42"/>
       <c r="E95" s="42"/>
       <c r="F95" s="42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G95" s="42" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H95" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I95" s="42" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J95" s="43"/>
     </row>
@@ -33139,13 +33157,13 @@
         <v>233</v>
       </c>
       <c r="G96" s="42" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H96" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I96" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J96" s="43"/>
     </row>
@@ -33163,13 +33181,13 @@
         <v>233</v>
       </c>
       <c r="G97" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H97" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I97" s="42" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J97" s="43"/>
     </row>
@@ -33187,13 +33205,13 @@
         <v>233</v>
       </c>
       <c r="G98" s="42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H98" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I98" s="42" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J98" s="43"/>
     </row>
@@ -33211,13 +33229,13 @@
         <v>233</v>
       </c>
       <c r="G99" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H99" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I99" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J99" s="43"/>
     </row>
@@ -33235,13 +33253,13 @@
         <v>233</v>
       </c>
       <c r="G100" s="42" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H100" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I100" s="42" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J100" s="43"/>
     </row>
@@ -33259,13 +33277,13 @@
         <v>233</v>
       </c>
       <c r="G101" s="42" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H101" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I101" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J101" s="43"/>
     </row>
@@ -33280,16 +33298,16 @@
       <c r="D102" s="42"/>
       <c r="E102" s="42"/>
       <c r="F102" s="42" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G102" s="42" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H102" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I102" s="42" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="J102" s="43"/>
     </row>
@@ -33307,13 +33325,13 @@
         <v>231</v>
       </c>
       <c r="G103" s="42" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H103" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I103" s="42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J103" s="43"/>
     </row>
@@ -33328,16 +33346,16 @@
       <c r="D104" s="42"/>
       <c r="E104" s="42"/>
       <c r="F104" s="42" t="s">
-        <v>2595</v>
+        <v>231</v>
       </c>
       <c r="G104" s="42" t="s">
-        <v>2596</v>
+        <v>237</v>
       </c>
       <c r="H104" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I104" s="42" t="s">
-        <v>2597</v>
+        <v>236</v>
       </c>
       <c r="J104" s="43"/>
     </row>
@@ -33355,13 +33373,13 @@
         <v>2595</v>
       </c>
       <c r="G105" s="42" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="H105" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I105" s="42" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="J105" s="43"/>
     </row>
@@ -33379,13 +33397,13 @@
         <v>2595</v>
       </c>
       <c r="G106" s="42" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="H106" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I106" s="42" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="J106" s="43"/>
     </row>
@@ -33403,13 +33421,13 @@
         <v>2595</v>
       </c>
       <c r="G107" s="42" t="s">
-        <v>2612</v>
+        <v>2600</v>
       </c>
       <c r="H107" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I107" s="42" t="s">
-        <v>2613</v>
+        <v>2601</v>
       </c>
       <c r="J107" s="43"/>
     </row>
@@ -33424,16 +33442,16 @@
       <c r="D108" s="42"/>
       <c r="E108" s="42"/>
       <c r="F108" s="42" t="s">
-        <v>238</v>
+        <v>2595</v>
       </c>
       <c r="G108" s="42" t="s">
-        <v>239</v>
+        <v>2612</v>
       </c>
       <c r="H108" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I108" s="42" t="s">
-        <v>240</v>
+        <v>2613</v>
       </c>
       <c r="J108" s="43"/>
     </row>
@@ -33448,16 +33466,16 @@
       <c r="D109" s="42"/>
       <c r="E109" s="42"/>
       <c r="F109" s="42" t="s">
-        <v>238</v>
+        <v>2595</v>
       </c>
       <c r="G109" s="42" t="s">
-        <v>241</v>
+        <v>2830</v>
       </c>
       <c r="H109" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I109" s="42" t="s">
-        <v>242</v>
+        <v>2831</v>
       </c>
       <c r="J109" s="43"/>
     </row>
@@ -33475,13 +33493,13 @@
         <v>238</v>
       </c>
       <c r="G110" s="42" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="H110" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I110" s="42" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J110" s="43"/>
     </row>
@@ -33499,13 +33517,13 @@
         <v>238</v>
       </c>
       <c r="G111" s="42" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H111" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I111" s="42" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="J111" s="43"/>
     </row>
@@ -33523,13 +33541,13 @@
         <v>238</v>
       </c>
       <c r="G112" s="42" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H112" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I112" s="42" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J112" s="43"/>
     </row>
@@ -33544,16 +33562,16 @@
       <c r="D113" s="42"/>
       <c r="E113" s="42"/>
       <c r="F113" s="42" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="G113" s="42" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H113" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I113" s="42" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="J113" s="43"/>
     </row>
@@ -33568,16 +33586,16 @@
       <c r="D114" s="42"/>
       <c r="E114" s="42"/>
       <c r="F114" s="42" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="G114" s="42" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="H114" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I114" s="42" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="J114" s="43"/>
     </row>
@@ -33595,13 +33613,13 @@
         <v>249</v>
       </c>
       <c r="G115" s="42" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H115" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I115" s="42" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J115" s="43"/>
     </row>
@@ -33619,13 +33637,13 @@
         <v>249</v>
       </c>
       <c r="G116" s="42" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="H116" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I116" s="42" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="J116" s="43"/>
     </row>
@@ -33643,13 +33661,13 @@
         <v>249</v>
       </c>
       <c r="G117" s="42" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="H117" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I117" s="42" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J117" s="43"/>
     </row>
@@ -33667,13 +33685,13 @@
         <v>249</v>
       </c>
       <c r="G118" s="42" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H118" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I118" s="42" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J118" s="43"/>
     </row>
@@ -33691,17 +33709,15 @@
         <v>249</v>
       </c>
       <c r="G119" s="42" t="s">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="H119" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I119" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="J119" s="43" t="s">
-        <v>102</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="J119" s="43"/>
     </row>
     <row r="120" spans="1:10" s="44" customFormat="1">
       <c r="A120" s="41" t="s">
@@ -33714,16 +33730,16 @@
       <c r="D120" s="42"/>
       <c r="E120" s="42"/>
       <c r="F120" s="42" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="G120" s="42" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H120" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I120" s="42" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J120" s="43"/>
     </row>
@@ -33732,46 +33748,48 @@
         <v>0</v>
       </c>
       <c r="B121" s="42" t="s">
-        <v>284</v>
+        <v>395</v>
       </c>
       <c r="C121" s="42"/>
       <c r="D121" s="42"/>
       <c r="E121" s="42"/>
       <c r="F121" s="42" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="G121" s="42" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H121" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I121" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="J121" s="43"/>
+        <v>261</v>
+      </c>
+      <c r="J121" s="43" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="122" spans="1:10" s="44" customFormat="1">
       <c r="A122" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B122" s="42" t="s">
-        <v>284</v>
+        <v>395</v>
       </c>
       <c r="C122" s="42"/>
       <c r="D122" s="42"/>
       <c r="E122" s="42"/>
       <c r="F122" s="42" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G122" s="42" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H122" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I122" s="42" t="s">
-        <v>2594</v>
+        <v>262</v>
       </c>
       <c r="J122" s="43"/>
     </row>
@@ -33789,13 +33807,13 @@
         <v>266</v>
       </c>
       <c r="G123" s="42" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H123" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I123" s="42" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J123" s="43"/>
     </row>
@@ -33813,13 +33831,13 @@
         <v>266</v>
       </c>
       <c r="G124" s="42" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H124" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I124" s="42" t="s">
-        <v>273</v>
+        <v>2594</v>
       </c>
       <c r="J124" s="43"/>
     </row>
@@ -33834,44 +33852,92 @@
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
       <c r="F125" s="42" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G125" s="42" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H125" s="42" t="s">
         <v>215</v>
       </c>
       <c r="I125" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="J125" s="43"/>
+    </row>
+    <row r="126" spans="1:10" s="44" customFormat="1">
+      <c r="A126" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="C126" s="42"/>
+      <c r="D126" s="42"/>
+      <c r="E126" s="42"/>
+      <c r="F126" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G126" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="H126" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="I126" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="J126" s="43"/>
+    </row>
+    <row r="127" spans="1:10" s="44" customFormat="1">
+      <c r="A127" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="C127" s="42"/>
+      <c r="D127" s="42"/>
+      <c r="E127" s="42"/>
+      <c r="F127" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="G127" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="H127" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="I127" s="42" t="s">
         <v>276</v>
       </c>
-      <c r="J125" s="43" t="s">
+      <c r="J127" s="43" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
-      <c r="A126" s="7" t="s">
+    <row r="128" spans="1:10">
+      <c r="A128" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B128" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C126" s="8"/>
-      <c r="D126" s="8"/>
-      <c r="E126" s="8"/>
-      <c r="F126" s="8" t="s">
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="G126" s="8" t="s">
+      <c r="G128" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="H126" s="8" t="s">
+      <c r="H128" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="I126" s="8" t="s">
+      <c r="I128" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="J126" s="10"/>
+      <c r="J128" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -36581,10 +36647,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -37338,7 +37404,7 @@
       <c r="H29" s="49" t="s">
         <v>1069</v>
       </c>
-      <c r="I29" s="64" t="s">
+      <c r="I29" s="56" t="s">
         <v>2732</v>
       </c>
       <c r="J29" s="50"/>
@@ -37838,7 +37904,7 @@
       <c r="B49" s="42"/>
       <c r="C49" s="49"/>
       <c r="D49" s="49"/>
-      <c r="E49" s="61" t="s">
+      <c r="E49" s="53" t="s">
         <v>2827</v>
       </c>
       <c r="F49" s="49"/>

</xml_diff>

<commit_message>
Atualização Controles Tabelas - Nova
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sequência Execução" sheetId="35" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10525" uniqueCount="2832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10562" uniqueCount="2842">
   <si>
     <t>Processo de Carga LN</t>
   </si>
@@ -8543,6 +8543,36 @@
   </si>
   <si>
     <t>ln.ods_wms_romaneio</t>
+  </si>
+  <si>
+    <t>Despesas_LN</t>
+  </si>
+  <si>
+    <t>(DFT) SKU Interno</t>
+  </si>
+  <si>
+    <t>(DFT) SKU - Departamento Interno</t>
+  </si>
+  <si>
+    <t>dbo.stg_sku_interno</t>
+  </si>
+  <si>
+    <t>dbo.stg_dom_sku_depto_interno</t>
+  </si>
+  <si>
+    <t>(SC) Estrutura Compra Ativo</t>
+  </si>
+  <si>
+    <t>(DFT) Departamento Interno</t>
+  </si>
+  <si>
+    <t>(DFT) Sku Interno</t>
+  </si>
+  <si>
+    <t>ln.ods_dom_sku_depto_interno</t>
+  </si>
+  <si>
+    <t>ln.ods_sku_interno</t>
   </si>
 </sst>
 </file>
@@ -19592,8 +19622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -30265,7 +30295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
     </sheetView>
@@ -36648,9 +36678,9 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -37873,15 +37903,6 @@
       <c r="A48" s="41" t="s">
         <v>2819</v>
       </c>
-      <c r="B48" s="42" t="s">
-        <v>2825</v>
-      </c>
-      <c r="C48" s="49" t="s">
-        <v>2824</v>
-      </c>
-      <c r="D48" s="49" t="s">
-        <v>2826</v>
-      </c>
       <c r="E48" s="49" t="s">
         <v>2820</v>
       </c>
@@ -37900,10 +37921,18 @@
       <c r="J48" s="50"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="41"/>
-      <c r="B49" s="42"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
+      <c r="A49" s="41" t="s">
+        <v>2832</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>2825</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>2824</v>
+      </c>
+      <c r="D49" s="49" t="s">
+        <v>2826</v>
+      </c>
       <c r="E49" s="53" t="s">
         <v>2827</v>
       </c>
@@ -38353,11 +38382,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M165"/>
+  <dimension ref="A1:M169"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I123" sqref="I123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -39608,70 +39637,58 @@
       <c r="M45" s="9"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="33" t="s">
-        <v>379</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>448</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>381</v>
-      </c>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33" t="s">
-        <v>396</v>
-      </c>
-      <c r="J46" s="33" t="s">
-        <v>397</v>
-      </c>
-      <c r="K46" s="33" t="s">
-        <v>398</v>
-      </c>
-      <c r="L46" s="33" t="s">
-        <v>399</v>
-      </c>
-      <c r="M46" s="39"/>
+      <c r="B46" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>2833</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>2835</v>
+      </c>
+      <c r="M46" s="9"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="33" t="s">
-        <v>379</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>448</v>
-      </c>
-      <c r="E47" s="33" t="s">
-        <v>381</v>
-      </c>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33" t="s">
-        <v>396</v>
-      </c>
-      <c r="J47" s="33" t="s">
-        <v>400</v>
-      </c>
-      <c r="K47" s="33" t="s">
-        <v>398</v>
-      </c>
-      <c r="L47" s="33" t="s">
-        <v>401</v>
-      </c>
-      <c r="M47" s="39"/>
+      <c r="B47" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>2834</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>2836</v>
+      </c>
+      <c r="M47" s="9"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="37" t="s">
@@ -39696,13 +39713,13 @@
         <v>396</v>
       </c>
       <c r="J48" s="33" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="K48" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L48" s="33" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="M48" s="39"/>
     </row>
@@ -39729,17 +39746,15 @@
         <v>396</v>
       </c>
       <c r="J49" s="33" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="K49" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L49" s="33" t="s">
-        <v>405</v>
-      </c>
-      <c r="M49" s="39" t="s">
-        <v>102</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="M49" s="39"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="37" t="s">
@@ -39764,13 +39779,13 @@
         <v>396</v>
       </c>
       <c r="J50" s="33" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="K50" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L50" s="33" t="s">
-        <v>2484</v>
+        <v>403</v>
       </c>
       <c r="M50" s="39"/>
     </row>
@@ -39797,15 +39812,17 @@
         <v>396</v>
       </c>
       <c r="J51" s="33" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="K51" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L51" s="33" t="s">
-        <v>407</v>
-      </c>
-      <c r="M51" s="39"/>
+        <v>405</v>
+      </c>
+      <c r="M51" s="39" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="37" t="s">
@@ -39830,13 +39847,13 @@
         <v>396</v>
       </c>
       <c r="J52" s="33" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K52" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L52" s="33" t="s">
-        <v>410</v>
+        <v>2484</v>
       </c>
       <c r="M52" s="39"/>
     </row>
@@ -39863,13 +39880,13 @@
         <v>396</v>
       </c>
       <c r="J53" s="33" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="K53" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L53" s="33" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="M53" s="39"/>
     </row>
@@ -39896,13 +39913,13 @@
         <v>396</v>
       </c>
       <c r="J54" s="33" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="K54" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L54" s="33" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="M54" s="39"/>
     </row>
@@ -39929,13 +39946,13 @@
         <v>396</v>
       </c>
       <c r="J55" s="33" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="K55" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L55" s="33" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="M55" s="39"/>
     </row>
@@ -39962,13 +39979,13 @@
         <v>396</v>
       </c>
       <c r="J56" s="33" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="K56" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L56" s="33" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M56" s="39"/>
     </row>
@@ -39995,13 +40012,13 @@
         <v>396</v>
       </c>
       <c r="J57" s="33" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="K57" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L57" s="33" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="M57" s="39"/>
     </row>
@@ -40028,13 +40045,13 @@
         <v>396</v>
       </c>
       <c r="J58" s="33" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="K58" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L58" s="33" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M58" s="39"/>
     </row>
@@ -40061,13 +40078,13 @@
         <v>396</v>
       </c>
       <c r="J59" s="33" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="K59" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L59" s="33" t="s">
-        <v>2616</v>
+        <v>420</v>
       </c>
       <c r="M59" s="39"/>
     </row>
@@ -40091,16 +40108,16 @@
       <c r="G60" s="33"/>
       <c r="H60" s="33"/>
       <c r="I60" s="33" t="s">
-        <v>2677</v>
+        <v>396</v>
       </c>
       <c r="J60" s="33" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="K60" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L60" s="33" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="M60" s="39"/>
     </row>
@@ -40124,16 +40141,16 @@
       <c r="G61" s="33"/>
       <c r="H61" s="33"/>
       <c r="I61" s="33" t="s">
-        <v>2677</v>
+        <v>396</v>
       </c>
       <c r="J61" s="33" t="s">
-        <v>2679</v>
+        <v>425</v>
       </c>
       <c r="K61" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L61" s="33" t="s">
-        <v>2678</v>
+        <v>2616</v>
       </c>
       <c r="M61" s="39"/>
     </row>
@@ -40160,13 +40177,13 @@
         <v>2677</v>
       </c>
       <c r="J62" s="33" t="s">
-        <v>2680</v>
+        <v>421</v>
       </c>
       <c r="K62" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L62" s="33" t="s">
-        <v>2681</v>
+        <v>422</v>
       </c>
       <c r="M62" s="39"/>
     </row>
@@ -40193,13 +40210,13 @@
         <v>2677</v>
       </c>
       <c r="J63" s="33" t="s">
-        <v>2682</v>
+        <v>2679</v>
       </c>
       <c r="K63" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L63" s="33" t="s">
-        <v>2683</v>
+        <v>2678</v>
       </c>
       <c r="M63" s="39"/>
     </row>
@@ -40226,13 +40243,13 @@
         <v>2677</v>
       </c>
       <c r="J64" s="33" t="s">
-        <v>2684</v>
+        <v>2680</v>
       </c>
       <c r="K64" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L64" s="33" t="s">
-        <v>2685</v>
+        <v>2681</v>
       </c>
       <c r="M64" s="39"/>
     </row>
@@ -40256,16 +40273,16 @@
       <c r="G65" s="33"/>
       <c r="H65" s="33"/>
       <c r="I65" s="33" t="s">
-        <v>426</v>
+        <v>2677</v>
       </c>
       <c r="J65" s="33" t="s">
-        <v>427</v>
+        <v>2682</v>
       </c>
       <c r="K65" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L65" s="33" t="s">
-        <v>428</v>
+        <v>2683</v>
       </c>
       <c r="M65" s="39"/>
     </row>
@@ -40289,16 +40306,16 @@
       <c r="G66" s="33"/>
       <c r="H66" s="33"/>
       <c r="I66" s="33" t="s">
-        <v>429</v>
+        <v>2677</v>
       </c>
       <c r="J66" s="33" t="s">
-        <v>430</v>
+        <v>2684</v>
       </c>
       <c r="K66" s="33" t="s">
         <v>398</v>
       </c>
       <c r="L66" s="33" t="s">
-        <v>431</v>
+        <v>2685</v>
       </c>
       <c r="M66" s="39"/>
     </row>
@@ -40313,25 +40330,25 @@
         <v>380</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E67" s="33" t="s">
-        <v>449</v>
+        <v>381</v>
       </c>
       <c r="F67" s="33"/>
       <c r="G67" s="33"/>
       <c r="H67" s="33"/>
       <c r="I67" s="33" t="s">
-        <v>2686</v>
+        <v>426</v>
       </c>
       <c r="J67" s="33" t="s">
-        <v>473</v>
+        <v>427</v>
       </c>
       <c r="K67" s="33" t="s">
-        <v>215</v>
+        <v>398</v>
       </c>
       <c r="L67" s="33" t="s">
-        <v>474</v>
+        <v>428</v>
       </c>
       <c r="M67" s="39"/>
     </row>
@@ -40346,25 +40363,25 @@
         <v>380</v>
       </c>
       <c r="D68" s="33" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E68" s="33" t="s">
-        <v>449</v>
+        <v>381</v>
       </c>
       <c r="F68" s="33"/>
       <c r="G68" s="33"/>
       <c r="H68" s="33"/>
       <c r="I68" s="33" t="s">
-        <v>2686</v>
+        <v>429</v>
       </c>
       <c r="J68" s="33" t="s">
-        <v>2679</v>
+        <v>430</v>
       </c>
       <c r="K68" s="33" t="s">
-        <v>215</v>
+        <v>398</v>
       </c>
       <c r="L68" s="33" t="s">
-        <v>2687</v>
+        <v>431</v>
       </c>
       <c r="M68" s="39"/>
     </row>
@@ -40391,13 +40408,13 @@
         <v>2686</v>
       </c>
       <c r="J69" s="33" t="s">
-        <v>2680</v>
+        <v>473</v>
       </c>
       <c r="K69" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L69" s="33" t="s">
-        <v>2688</v>
+        <v>474</v>
       </c>
       <c r="M69" s="39"/>
     </row>
@@ -40424,13 +40441,13 @@
         <v>2686</v>
       </c>
       <c r="J70" s="33" t="s">
-        <v>2682</v>
+        <v>2679</v>
       </c>
       <c r="K70" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L70" s="33" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
       <c r="M70" s="39"/>
     </row>
@@ -40457,13 +40474,13 @@
         <v>2686</v>
       </c>
       <c r="J71" s="33" t="s">
-        <v>2684</v>
+        <v>2680</v>
       </c>
       <c r="K71" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L71" s="33" t="s">
-        <v>2690</v>
+        <v>2688</v>
       </c>
       <c r="M71" s="39"/>
     </row>
@@ -40487,16 +40504,16 @@
       <c r="G72" s="33"/>
       <c r="H72" s="33"/>
       <c r="I72" s="33" t="s">
-        <v>450</v>
+        <v>2686</v>
       </c>
       <c r="J72" s="33" t="s">
-        <v>451</v>
+        <v>2682</v>
       </c>
       <c r="K72" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L72" s="33" t="s">
-        <v>452</v>
+        <v>2689</v>
       </c>
       <c r="M72" s="39"/>
     </row>
@@ -40520,16 +40537,16 @@
       <c r="G73" s="33"/>
       <c r="H73" s="33"/>
       <c r="I73" s="33" t="s">
-        <v>450</v>
+        <v>2686</v>
       </c>
       <c r="J73" s="33" t="s">
-        <v>453</v>
+        <v>2684</v>
       </c>
       <c r="K73" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L73" s="33" t="s">
-        <v>454</v>
+        <v>2690</v>
       </c>
       <c r="M73" s="39"/>
     </row>
@@ -40556,13 +40573,13 @@
         <v>450</v>
       </c>
       <c r="J74" s="33" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="K74" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L74" s="33" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="M74" s="39"/>
     </row>
@@ -40589,13 +40606,13 @@
         <v>450</v>
       </c>
       <c r="J75" s="33" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K75" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L75" s="33" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="M75" s="39"/>
     </row>
@@ -40619,16 +40636,16 @@
       <c r="G76" s="33"/>
       <c r="H76" s="33"/>
       <c r="I76" s="33" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="J76" s="33" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="K76" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L76" s="33" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="M76" s="39"/>
     </row>
@@ -40652,16 +40669,16 @@
       <c r="G77" s="33"/>
       <c r="H77" s="33"/>
       <c r="I77" s="33" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="J77" s="33" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="K77" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L77" s="33" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="M77" s="39"/>
     </row>
@@ -40688,13 +40705,13 @@
         <v>458</v>
       </c>
       <c r="J78" s="33" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="K78" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L78" s="33" t="s">
-        <v>2485</v>
+        <v>460</v>
       </c>
       <c r="M78" s="39"/>
     </row>
@@ -40721,13 +40738,13 @@
         <v>458</v>
       </c>
       <c r="J79" s="33" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="K79" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L79" s="33" t="s">
-        <v>2617</v>
+        <v>461</v>
       </c>
       <c r="M79" s="39"/>
     </row>
@@ -40754,13 +40771,13 @@
         <v>458</v>
       </c>
       <c r="J80" s="33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K80" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L80" s="33" t="s">
-        <v>464</v>
+        <v>2485</v>
       </c>
       <c r="M80" s="39"/>
     </row>
@@ -40787,13 +40804,13 @@
         <v>458</v>
       </c>
       <c r="J81" s="33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K81" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L81" s="33" t="s">
-        <v>465</v>
+        <v>2617</v>
       </c>
       <c r="M81" s="39"/>
     </row>
@@ -40820,13 +40837,13 @@
         <v>458</v>
       </c>
       <c r="J82" s="33" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="K82" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L82" s="33" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="M82" s="39"/>
     </row>
@@ -40853,13 +40870,13 @@
         <v>458</v>
       </c>
       <c r="J83" s="33" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="K83" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L83" s="33" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="M83" s="39"/>
     </row>
@@ -40886,17 +40903,15 @@
         <v>458</v>
       </c>
       <c r="J84" s="33" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="K84" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L84" s="33" t="s">
-        <v>2618</v>
-      </c>
-      <c r="M84" s="39" t="s">
-        <v>102</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="M84" s="39"/>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="37" t="s">
@@ -40921,17 +40936,15 @@
         <v>458</v>
       </c>
       <c r="J85" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K85" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L85" s="33" t="s">
-        <v>2619</v>
-      </c>
-      <c r="M85" s="39" t="s">
-        <v>102</v>
-      </c>
+        <v>469</v>
+      </c>
+      <c r="M85" s="39"/>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="37" t="s">
@@ -40956,15 +40969,17 @@
         <v>458</v>
       </c>
       <c r="J86" s="33" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K86" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L86" s="33" t="s">
-        <v>472</v>
-      </c>
-      <c r="M86" s="39"/>
+        <v>2618</v>
+      </c>
+      <c r="M86" s="39" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="37" t="s">
@@ -40989,15 +41004,17 @@
         <v>458</v>
       </c>
       <c r="J87" s="33" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="K87" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L87" s="33" t="s">
-        <v>474</v>
-      </c>
-      <c r="M87" s="39"/>
+        <v>2619</v>
+      </c>
+      <c r="M87" s="39" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="37" t="s">
@@ -41019,16 +41036,16 @@
       <c r="G88" s="33"/>
       <c r="H88" s="33"/>
       <c r="I88" s="33" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="J88" s="33" t="s">
-        <v>413</v>
+        <v>471</v>
       </c>
       <c r="K88" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L88" s="33" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="M88" s="39"/>
     </row>
@@ -41052,16 +41069,16 @@
       <c r="G89" s="33"/>
       <c r="H89" s="33"/>
       <c r="I89" s="33" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="J89" s="33" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="K89" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L89" s="33" t="s">
-        <v>2486</v>
+        <v>474</v>
       </c>
       <c r="M89" s="39"/>
     </row>
@@ -41088,13 +41105,13 @@
         <v>475</v>
       </c>
       <c r="J90" s="33" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="K90" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L90" s="33" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="M90" s="39"/>
     </row>
@@ -41121,13 +41138,13 @@
         <v>475</v>
       </c>
       <c r="J91" s="33" t="s">
-        <v>415</v>
+        <v>477</v>
       </c>
       <c r="K91" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L91" s="33" t="s">
-        <v>479</v>
+        <v>2486</v>
       </c>
       <c r="M91" s="39"/>
     </row>
@@ -41154,13 +41171,13 @@
         <v>475</v>
       </c>
       <c r="J92" s="33" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K92" s="33" t="s">
         <v>215</v>
       </c>
       <c r="L92" s="33" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="M92" s="39"/>
     </row>
@@ -41187,13 +41204,13 @@
         <v>475</v>
       </c>
       <c r="J93" s="33" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="K93" s="33" t="s">
-        <v>488</v>
+        <v>215</v>
       </c>
       <c r="L93" s="33" t="s">
-        <v>692</v>
+        <v>479</v>
       </c>
       <c r="M93" s="39"/>
     </row>
@@ -41202,25 +41219,31 @@
         <v>0</v>
       </c>
       <c r="B94" s="33" t="s">
-        <v>434</v>
-      </c>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
+        <v>379</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="D94" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="E94" s="33" t="s">
+        <v>449</v>
+      </c>
       <c r="F94" s="33"/>
       <c r="G94" s="33"/>
       <c r="H94" s="33"/>
       <c r="I94" s="33" t="s">
-        <v>435</v>
+        <v>475</v>
       </c>
       <c r="J94" s="33" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="K94" s="33" t="s">
-        <v>6</v>
+        <v>215</v>
       </c>
       <c r="L94" s="33" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="M94" s="39"/>
     </row>
@@ -41229,25 +41252,31 @@
         <v>0</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>434</v>
-      </c>
-      <c r="C95" s="33"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="33"/>
+        <v>379</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="D95" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>449</v>
+      </c>
       <c r="F95" s="33"/>
       <c r="G95" s="33"/>
       <c r="H95" s="33"/>
       <c r="I95" s="33" t="s">
-        <v>435</v>
+        <v>475</v>
       </c>
       <c r="J95" s="33" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="K95" s="33" t="s">
-        <v>6</v>
+        <v>488</v>
       </c>
       <c r="L95" s="33" t="s">
-        <v>439</v>
+        <v>692</v>
       </c>
       <c r="M95" s="39"/>
     </row>
@@ -41268,93 +41297,69 @@
         <v>435</v>
       </c>
       <c r="J96" s="33" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="K96" s="33" t="s">
         <v>6</v>
       </c>
       <c r="L96" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="M96" s="39"/>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="C97" s="33"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="33"/>
+      <c r="G97" s="33"/>
+      <c r="H97" s="33"/>
+      <c r="I97" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="J97" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="K97" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L97" s="33" t="s">
+        <v>439</v>
+      </c>
+      <c r="M97" s="39"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="33"/>
+      <c r="H98" s="33"/>
+      <c r="I98" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="J98" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="K98" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L98" s="33" t="s">
         <v>441</v>
       </c>
-      <c r="M96" s="39"/>
-    </row>
-    <row r="97" spans="1:13" ht="12.75">
-      <c r="A97" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B97" s="13" t="s">
-        <v>444</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="H97" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="I97" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="J97" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="K97" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="L97" s="42" t="s">
-        <v>489</v>
-      </c>
-      <c r="M97" s="9"/>
-    </row>
-    <row r="98" spans="1:13" ht="12.75">
-      <c r="A98" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B98" s="13" t="s">
-        <v>444</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="G98" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="H98" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="I98" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="J98" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="K98" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="L98" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="M98" s="9"/>
+      <c r="M98" s="39"/>
     </row>
     <row r="99" spans="1:13" ht="12.75">
       <c r="A99" s="5" t="s">
@@ -41376,22 +41381,22 @@
         <v>483</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="J99" s="6" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="K99" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="L99" s="6" t="s">
-        <v>496</v>
+      <c r="L99" s="42" t="s">
+        <v>489</v>
       </c>
       <c r="M99" s="9"/>
     </row>
@@ -41424,13 +41429,13 @@
         <v>492</v>
       </c>
       <c r="J100" s="6" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="K100" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L100" s="6" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="M100" s="9"/>
     </row>
@@ -41463,13 +41468,13 @@
         <v>492</v>
       </c>
       <c r="J101" s="6" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="K101" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L101" s="6" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="M101" s="9"/>
     </row>
@@ -41493,22 +41498,22 @@
         <v>483</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="J102" s="6" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="K102" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L102" s="6" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="M102" s="9"/>
     </row>
@@ -41532,22 +41537,22 @@
         <v>483</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="K103" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L103" s="6" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="M103" s="9"/>
     </row>
@@ -41580,13 +41585,13 @@
         <v>503</v>
       </c>
       <c r="J104" s="6" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="K104" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="M104" s="9"/>
     </row>
@@ -41601,25 +41606,31 @@
         <v>446</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
+        <v>482</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H105" s="6" t="s">
+        <v>502</v>
+      </c>
       <c r="I105" s="6" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="J105" s="6" t="s">
-        <v>309</v>
+        <v>497</v>
       </c>
       <c r="K105" s="6" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="M105" s="9"/>
     </row>
@@ -41634,25 +41645,31 @@
         <v>446</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>512</v>
+        <v>481</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="6"/>
+        <v>482</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>502</v>
+      </c>
       <c r="I106" s="6" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="J106" s="6" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="K106" s="6" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="L106" s="6" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="M106" s="9"/>
     </row>
@@ -41667,25 +41684,25 @@
         <v>446</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
       <c r="H107" s="6"/>
       <c r="I107" s="6" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="J107" s="6" t="s">
-        <v>520</v>
+        <v>309</v>
       </c>
       <c r="K107" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="M107" s="9"/>
     </row>
@@ -41700,31 +41717,25 @@
         <v>446</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="H108" s="6" t="s">
-        <v>525</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
       <c r="I108" s="6" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="J108" s="6" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="K108" s="6" t="s">
-        <v>398</v>
+        <v>511</v>
       </c>
       <c r="L108" s="6" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="M108" s="9"/>
     </row>
@@ -41739,31 +41750,25 @@
         <v>446</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F109" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="H109" s="6" t="s">
-        <v>529</v>
-      </c>
+        <v>518</v>
+      </c>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
       <c r="I109" s="6" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="J109" s="6" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="K109" s="6" t="s">
-        <v>215</v>
+        <v>511</v>
       </c>
       <c r="L109" s="6" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="M109" s="9"/>
     </row>
@@ -41778,31 +41783,31 @@
         <v>446</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>484</v>
       </c>
       <c r="H110" s="6" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="I110" s="6" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
       <c r="J110" s="6" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="K110" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="M110" s="9"/>
     </row>
@@ -41817,31 +41822,31 @@
         <v>446</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="I111" s="6" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="J111" s="6" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>398</v>
+        <v>215</v>
       </c>
       <c r="L111" s="6" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="M111" s="9"/>
     </row>
@@ -41874,13 +41879,13 @@
         <v>536</v>
       </c>
       <c r="J112" s="6" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="K112" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="M112" s="9"/>
     </row>
@@ -41913,13 +41918,13 @@
         <v>536</v>
       </c>
       <c r="J113" s="6" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="K113" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L113" s="6" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="M113" s="9"/>
     </row>
@@ -41952,13 +41957,13 @@
         <v>536</v>
       </c>
       <c r="J114" s="6" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="K114" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="M114" s="9"/>
     </row>
@@ -41991,13 +41996,13 @@
         <v>536</v>
       </c>
       <c r="J115" s="6" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="K115" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="M115" s="9"/>
     </row>
@@ -42030,13 +42035,13 @@
         <v>536</v>
       </c>
       <c r="J116" s="6" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="K116" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="M116" s="9"/>
     </row>
@@ -42069,13 +42074,13 @@
         <v>536</v>
       </c>
       <c r="J117" s="6" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="K117" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="M117" s="9"/>
     </row>
@@ -42108,13 +42113,13 @@
         <v>536</v>
       </c>
       <c r="J118" s="6" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="K118" s="6" t="s">
         <v>398</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="M118" s="9"/>
     </row>
@@ -42147,13 +42152,13 @@
         <v>536</v>
       </c>
       <c r="J119" s="6" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="K119" s="6" t="s">
-        <v>488</v>
+        <v>398</v>
       </c>
       <c r="L119" s="6" t="s">
-        <v>2620</v>
+        <v>552</v>
       </c>
       <c r="M119" s="9"/>
     </row>
@@ -42177,22 +42182,22 @@
         <v>534</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="I120" s="6" t="s">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="J120" s="6" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="K120" s="6" t="s">
-        <v>511</v>
+        <v>398</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="M120" s="9"/>
     </row>
@@ -42216,22 +42221,22 @@
         <v>534</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="I121" s="6" t="s">
-        <v>560</v>
+        <v>536</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="K121" s="6" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="L121" s="6" t="s">
-        <v>562</v>
+        <v>2620</v>
       </c>
       <c r="M121" s="9"/>
     </row>
@@ -42261,16 +42266,16 @@
         <v>556</v>
       </c>
       <c r="I122" s="6" t="s">
-        <v>560</v>
+        <v>2837</v>
       </c>
       <c r="J122" s="6" t="s">
-        <v>563</v>
+        <v>2838</v>
       </c>
       <c r="K122" s="6" t="s">
-        <v>511</v>
+        <v>215</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>564</v>
+        <v>2840</v>
       </c>
       <c r="M122" s="9"/>
     </row>
@@ -42300,16 +42305,16 @@
         <v>556</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>560</v>
+        <v>2837</v>
       </c>
       <c r="J123" s="6" t="s">
-        <v>565</v>
+        <v>2839</v>
       </c>
       <c r="K123" s="6" t="s">
-        <v>511</v>
+        <v>215</v>
       </c>
       <c r="L123" s="6" t="s">
-        <v>566</v>
+        <v>2841</v>
       </c>
       <c r="M123" s="9"/>
     </row>
@@ -42339,16 +42344,16 @@
         <v>556</v>
       </c>
       <c r="I124" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="J124" s="6" t="s">
-        <v>549</v>
+        <v>558</v>
       </c>
       <c r="K124" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="M124" s="9"/>
     </row>
@@ -42381,13 +42386,13 @@
         <v>560</v>
       </c>
       <c r="J125" s="6" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="K125" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="M125" s="9"/>
     </row>
@@ -42420,13 +42425,13 @@
         <v>560</v>
       </c>
       <c r="J126" s="6" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="K126" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="M126" s="9"/>
     </row>
@@ -42459,13 +42464,13 @@
         <v>560</v>
       </c>
       <c r="J127" s="6" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="K127" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L127" s="6" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="M127" s="9"/>
     </row>
@@ -42498,7 +42503,7 @@
         <v>560</v>
       </c>
       <c r="J128" s="6" t="s">
-        <v>572</v>
+        <v>549</v>
       </c>
       <c r="K128" s="6" t="s">
         <v>511</v>
@@ -42537,13 +42542,13 @@
         <v>560</v>
       </c>
       <c r="J129" s="6" t="s">
-        <v>573</v>
+        <v>549</v>
       </c>
       <c r="K129" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L129" s="6" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="M129" s="9"/>
     </row>
@@ -42576,7 +42581,7 @@
         <v>560</v>
       </c>
       <c r="J130" s="6" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="K130" s="6" t="s">
         <v>511</v>
@@ -42615,13 +42620,13 @@
         <v>560</v>
       </c>
       <c r="J131" s="6" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="K131" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="M131" s="9"/>
     </row>
@@ -42654,7 +42659,7 @@
         <v>560</v>
       </c>
       <c r="J132" s="6" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="K132" s="6" t="s">
         <v>511</v>
@@ -42684,22 +42689,22 @@
         <v>534</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>578</v>
+        <v>556</v>
       </c>
       <c r="I133" s="6" t="s">
-        <v>503</v>
+        <v>560</v>
       </c>
       <c r="J133" s="6" t="s">
-        <v>549</v>
+        <v>573</v>
       </c>
       <c r="K133" s="6" t="s">
-        <v>488</v>
+        <v>511</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="M133" s="9"/>
     </row>
@@ -42723,22 +42728,22 @@
         <v>534</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="H134" s="6" t="s">
-        <v>578</v>
+        <v>556</v>
       </c>
       <c r="I134" s="6" t="s">
-        <v>503</v>
+        <v>560</v>
       </c>
       <c r="J134" s="6" t="s">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="K134" s="6" t="s">
-        <v>488</v>
+        <v>511</v>
       </c>
       <c r="L134" s="6" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="M134" s="9"/>
     </row>
@@ -42762,22 +42767,22 @@
         <v>534</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>578</v>
+        <v>556</v>
       </c>
       <c r="I135" s="6" t="s">
-        <v>503</v>
+        <v>560</v>
       </c>
       <c r="J135" s="6" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="K135" s="6" t="s">
-        <v>488</v>
+        <v>511</v>
       </c>
       <c r="L135" s="6" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="M135" s="9"/>
     </row>
@@ -42792,31 +42797,31 @@
         <v>446</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>582</v>
+        <v>532</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>583</v>
+        <v>533</v>
       </c>
       <c r="F136" s="6" t="s">
-        <v>584</v>
+        <v>534</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="H136" s="6" t="s">
-        <v>585</v>
+        <v>556</v>
       </c>
       <c r="I136" s="6" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="J136" s="6" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="K136" s="6" t="s">
-        <v>488</v>
+        <v>511</v>
       </c>
       <c r="L136" s="6" t="s">
-        <v>588</v>
+        <v>567</v>
       </c>
       <c r="M136" s="9"/>
     </row>
@@ -42831,31 +42836,31 @@
         <v>446</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>582</v>
+        <v>532</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>583</v>
+        <v>533</v>
       </c>
       <c r="F137" s="6" t="s">
-        <v>584</v>
+        <v>534</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="H137" s="6" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="I137" s="6" t="s">
-        <v>590</v>
+        <v>503</v>
       </c>
       <c r="J137" s="6" t="s">
-        <v>587</v>
+        <v>549</v>
       </c>
       <c r="K137" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L137" s="6" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="M137" s="9"/>
     </row>
@@ -42870,31 +42875,31 @@
         <v>446</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>582</v>
+        <v>532</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>583</v>
+        <v>533</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>584</v>
+        <v>534</v>
       </c>
       <c r="G138" s="6" t="s">
         <v>501</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="I138" s="6" t="s">
-        <v>593</v>
+        <v>503</v>
       </c>
       <c r="J138" s="6" t="s">
-        <v>587</v>
+        <v>549</v>
       </c>
       <c r="K138" s="6" t="s">
         <v>488</v>
       </c>
       <c r="L138" s="6" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="M138" s="9"/>
     </row>
@@ -42909,25 +42914,31 @@
         <v>446</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>595</v>
+        <v>532</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>596</v>
-      </c>
-      <c r="F139" s="6"/>
-      <c r="G139" s="6"/>
-      <c r="H139" s="6"/>
+        <v>533</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="G139" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H139" s="6" t="s">
+        <v>578</v>
+      </c>
       <c r="I139" s="6" t="s">
-        <v>597</v>
+        <v>503</v>
       </c>
       <c r="J139" s="6" t="s">
-        <v>357</v>
+        <v>581</v>
       </c>
       <c r="K139" s="6" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="L139" s="6" t="s">
-        <v>598</v>
+        <v>579</v>
       </c>
       <c r="M139" s="9"/>
     </row>
@@ -42942,25 +42953,31 @@
         <v>446</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>599</v>
+        <v>582</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>600</v>
-      </c>
-      <c r="F140" s="6"/>
-      <c r="G140" s="6"/>
-      <c r="H140" s="6"/>
+        <v>583</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>585</v>
+      </c>
       <c r="I140" s="6" t="s">
-        <v>601</v>
+        <v>586</v>
       </c>
       <c r="J140" s="6" t="s">
-        <v>82</v>
+        <v>587</v>
       </c>
       <c r="K140" s="6" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="L140" s="6" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="M140" s="9"/>
     </row>
@@ -42975,25 +42992,31 @@
         <v>446</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>599</v>
+        <v>582</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>600</v>
-      </c>
-      <c r="F141" s="6"/>
-      <c r="G141" s="6"/>
-      <c r="H141" s="6"/>
+        <v>583</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="G141" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="H141" s="6" t="s">
+        <v>589</v>
+      </c>
       <c r="I141" s="6" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="J141" s="6" t="s">
-        <v>82</v>
+        <v>587</v>
       </c>
       <c r="K141" s="6" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="L141" s="6" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="M141" s="9"/>
     </row>
@@ -43008,25 +43031,31 @@
         <v>446</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>605</v>
+        <v>582</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>604</v>
-      </c>
-      <c r="F142" s="6"/>
-      <c r="G142" s="6"/>
-      <c r="H142" s="6"/>
+        <v>583</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H142" s="6" t="s">
+        <v>592</v>
+      </c>
       <c r="I142" s="6" t="s">
-        <v>616</v>
+        <v>593</v>
       </c>
       <c r="J142" s="6" t="s">
-        <v>606</v>
+        <v>587</v>
       </c>
       <c r="K142" s="6" t="s">
-        <v>215</v>
+        <v>488</v>
       </c>
       <c r="L142" s="6" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="M142" s="9"/>
     </row>
@@ -43041,25 +43070,25 @@
         <v>446</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
       <c r="H143" s="6"/>
       <c r="I143" s="6" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="J143" s="6" t="s">
-        <v>611</v>
+        <v>357</v>
       </c>
       <c r="K143" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L143" s="6" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="M143" s="9"/>
     </row>
@@ -43074,25 +43103,25 @@
         <v>446</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
       <c r="H144" s="6"/>
       <c r="I144" s="6" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="J144" s="6" t="s">
-        <v>617</v>
+        <v>82</v>
       </c>
       <c r="K144" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L144" s="6" t="s">
-        <v>618</v>
+        <v>602</v>
       </c>
       <c r="M144" s="9"/>
     </row>
@@ -43107,25 +43136,25 @@
         <v>446</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="6"/>
       <c r="H145" s="6"/>
       <c r="I145" s="6" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="J145" s="6" t="s">
-        <v>622</v>
+        <v>82</v>
       </c>
       <c r="K145" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L145" s="6" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="M145" s="9"/>
     </row>
@@ -43140,25 +43169,25 @@
         <v>446</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>624</v>
+        <v>605</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>625</v>
+        <v>604</v>
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="6"/>
       <c r="H146" s="6"/>
       <c r="I146" s="6" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
       <c r="J146" s="6" t="s">
-        <v>627</v>
+        <v>606</v>
       </c>
       <c r="K146" s="6" t="s">
-        <v>511</v>
+        <v>215</v>
       </c>
       <c r="L146" s="6" t="s">
-        <v>626</v>
+        <v>607</v>
       </c>
       <c r="M146" s="9"/>
     </row>
@@ -43173,25 +43202,25 @@
         <v>446</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>629</v>
+        <v>608</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>630</v>
+        <v>609</v>
       </c>
       <c r="F147" s="6"/>
       <c r="G147" s="6"/>
       <c r="H147" s="6"/>
       <c r="I147" s="6" t="s">
-        <v>631</v>
+        <v>610</v>
       </c>
       <c r="J147" s="6" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
       <c r="K147" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L147" s="6" t="s">
-        <v>633</v>
+        <v>612</v>
       </c>
       <c r="M147" s="9"/>
     </row>
@@ -43206,25 +43235,25 @@
         <v>446</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>634</v>
+        <v>613</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>635</v>
+        <v>614</v>
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
       <c r="H148" s="6"/>
       <c r="I148" s="6" t="s">
-        <v>636</v>
+        <v>615</v>
       </c>
       <c r="J148" s="6" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="K148" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L148" s="6" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
       <c r="M148" s="9"/>
     </row>
@@ -43239,25 +43268,25 @@
         <v>446</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>639</v>
+        <v>619</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>640</v>
+        <v>620</v>
       </c>
       <c r="F149" s="6"/>
       <c r="G149" s="6"/>
       <c r="H149" s="6"/>
       <c r="I149" s="6" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="J149" s="6" t="s">
-        <v>355</v>
+        <v>622</v>
       </c>
       <c r="K149" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L149" s="6" t="s">
-        <v>642</v>
+        <v>623</v>
       </c>
       <c r="M149" s="9"/>
     </row>
@@ -43272,25 +43301,25 @@
         <v>446</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>643</v>
+        <v>624</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>644</v>
+        <v>625</v>
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="6"/>
       <c r="H150" s="6"/>
       <c r="I150" s="6" t="s">
-        <v>645</v>
+        <v>628</v>
       </c>
       <c r="J150" s="6" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="K150" s="6" t="s">
         <v>511</v>
       </c>
       <c r="L150" s="6" t="s">
-        <v>647</v>
+        <v>626</v>
       </c>
       <c r="M150" s="9"/>
     </row>
@@ -43305,25 +43334,25 @@
         <v>446</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>679</v>
+        <v>629</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>648</v>
+        <v>630</v>
       </c>
       <c r="F151" s="6"/>
       <c r="G151" s="6"/>
       <c r="H151" s="6"/>
       <c r="I151" s="6" t="s">
-        <v>649</v>
+        <v>631</v>
       </c>
       <c r="J151" s="6" t="s">
-        <v>650</v>
+        <v>632</v>
       </c>
       <c r="K151" s="6" t="s">
-        <v>215</v>
+        <v>511</v>
       </c>
       <c r="L151" s="6" t="s">
-        <v>364</v>
+        <v>633</v>
       </c>
       <c r="M151" s="9"/>
     </row>
@@ -43338,25 +43367,25 @@
         <v>446</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>680</v>
+        <v>634</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>651</v>
+        <v>635</v>
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
       <c r="H152" s="6"/>
       <c r="I152" s="6" t="s">
-        <v>652</v>
+        <v>636</v>
       </c>
       <c r="J152" s="6" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K152" s="6" t="s">
-        <v>215</v>
+        <v>511</v>
       </c>
       <c r="L152" s="6" t="s">
-        <v>2621</v>
+        <v>638</v>
       </c>
       <c r="M152" s="9"/>
     </row>
@@ -43371,25 +43400,25 @@
         <v>446</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>681</v>
+        <v>639</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>654</v>
+        <v>640</v>
       </c>
       <c r="F153" s="6"/>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>
       <c r="I153" s="6" t="s">
-        <v>655</v>
+        <v>641</v>
       </c>
       <c r="J153" s="6" t="s">
-        <v>656</v>
+        <v>355</v>
       </c>
       <c r="K153" s="6" t="s">
-        <v>215</v>
+        <v>511</v>
       </c>
       <c r="L153" s="6" t="s">
-        <v>657</v>
+        <v>642</v>
       </c>
       <c r="M153" s="9"/>
     </row>
@@ -43404,25 +43433,25 @@
         <v>446</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>682</v>
+        <v>643</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>658</v>
+        <v>644</v>
       </c>
       <c r="F154" s="6"/>
       <c r="G154" s="6"/>
       <c r="H154" s="6"/>
       <c r="I154" s="6" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="J154" s="6" t="s">
-        <v>660</v>
+        <v>646</v>
       </c>
       <c r="K154" s="6" t="s">
-        <v>215</v>
+        <v>511</v>
       </c>
       <c r="L154" s="6" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="M154" s="9"/>
     </row>
@@ -43437,25 +43466,25 @@
         <v>446</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
       <c r="H155" s="6"/>
       <c r="I155" s="6" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
       <c r="J155" s="6" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="K155" s="6" t="s">
         <v>215</v>
       </c>
       <c r="L155" s="6" t="s">
-        <v>665</v>
+        <v>364</v>
       </c>
       <c r="M155" s="9"/>
     </row>
@@ -43470,25 +43499,25 @@
         <v>446</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
       <c r="H156" s="6"/>
       <c r="I156" s="6" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
       <c r="J156" s="6" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="K156" s="6" t="s">
         <v>215</v>
       </c>
       <c r="L156" s="6" t="s">
-        <v>669</v>
+        <v>2621</v>
       </c>
       <c r="M156" s="9"/>
     </row>
@@ -43503,25 +43532,25 @@
         <v>446</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="F157" s="6"/>
       <c r="G157" s="6"/>
       <c r="H157" s="6"/>
       <c r="I157" s="6" t="s">
-        <v>671</v>
+        <v>655</v>
       </c>
       <c r="J157" s="6" t="s">
-        <v>672</v>
+        <v>656</v>
       </c>
       <c r="K157" s="6" t="s">
-        <v>511</v>
+        <v>215</v>
       </c>
       <c r="L157" s="6" t="s">
-        <v>673</v>
+        <v>657</v>
       </c>
       <c r="M157" s="9"/>
     </row>
@@ -43536,25 +43565,25 @@
         <v>446</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="6"/>
       <c r="H158" s="6"/>
       <c r="I158" s="6" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
       <c r="J158" s="6" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
       <c r="K158" s="6" t="s">
-        <v>511</v>
+        <v>215</v>
       </c>
       <c r="L158" s="6" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="M158" s="9"/>
     </row>
@@ -43569,31 +43598,25 @@
         <v>446</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>687</v>
-      </c>
-      <c r="F159" s="6" t="s">
-        <v>688</v>
-      </c>
-      <c r="G159" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="H159" s="6" t="s">
-        <v>689</v>
-      </c>
+        <v>662</v>
+      </c>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
       <c r="I159" s="6" t="s">
-        <v>690</v>
+        <v>663</v>
       </c>
       <c r="J159" s="6" t="s">
-        <v>691</v>
+        <v>664</v>
       </c>
       <c r="K159" s="6" t="s">
-        <v>488</v>
+        <v>215</v>
       </c>
       <c r="L159" s="6" t="s">
-        <v>692</v>
+        <v>665</v>
       </c>
       <c r="M159" s="9"/>
     </row>
@@ -43608,198 +43631,336 @@
         <v>446</v>
       </c>
       <c r="D160" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>666</v>
+      </c>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="J160" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="K160" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L160" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="M160" s="9"/>
+    </row>
+    <row r="161" spans="1:13" ht="12.75">
+      <c r="A161" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B161" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D161" s="6" t="s">
+        <v>685</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="J161" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="K161" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="L161" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="M161" s="9"/>
+    </row>
+    <row r="162" spans="1:13" ht="12.75">
+      <c r="A162" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B162" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>686</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="J162" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="K162" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="L162" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="M162" s="9"/>
+    </row>
+    <row r="163" spans="1:13" ht="12.75">
+      <c r="A163" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B163" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D163" s="6" t="s">
         <v>678</v>
       </c>
-      <c r="E160" s="6" t="s">
+      <c r="E163" s="6" t="s">
         <v>687</v>
       </c>
-      <c r="F160" s="6" t="s">
+      <c r="F163" s="6" t="s">
         <v>688</v>
       </c>
-      <c r="G160" s="6" t="s">
+      <c r="G163" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="H163" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="I163" s="6" t="s">
+        <v>690</v>
+      </c>
+      <c r="J163" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="K163" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="L163" s="6" t="s">
+        <v>692</v>
+      </c>
+      <c r="M163" s="9"/>
+    </row>
+    <row r="164" spans="1:13" ht="12.75">
+      <c r="A164" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="E164" s="6" t="s">
+        <v>687</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="G164" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="H160" s="6" t="s">
+      <c r="H164" s="6" t="s">
         <v>693</v>
       </c>
-      <c r="I160" s="6" t="s">
+      <c r="I164" s="6" t="s">
         <v>694</v>
       </c>
-      <c r="J160" s="6" t="s">
+      <c r="J164" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="K160" s="6" t="s">
+      <c r="K164" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="L160" s="6" t="s">
+      <c r="L164" s="6" t="s">
         <v>695</v>
       </c>
-      <c r="M160" s="9"/>
-    </row>
-    <row r="161" spans="1:13" ht="12.75">
-      <c r="A161" s="15" t="s">
+      <c r="M164" s="9"/>
+    </row>
+    <row r="165" spans="1:13" ht="12.75">
+      <c r="A165" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="B161" s="51" t="s">
+      <c r="B165" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="C161" s="16" t="s">
+      <c r="C165" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="D161" s="16" t="s">
+      <c r="D165" s="16" t="s">
         <v>696</v>
       </c>
-      <c r="E161" s="16" t="s">
+      <c r="E165" s="16" t="s">
         <v>697</v>
       </c>
-      <c r="F161" s="16"/>
-      <c r="G161" s="16"/>
-      <c r="H161" s="16"/>
-      <c r="I161" s="16" t="s">
+      <c r="F165" s="16"/>
+      <c r="G165" s="16"/>
+      <c r="H165" s="16"/>
+      <c r="I165" s="16" t="s">
         <v>698</v>
       </c>
-      <c r="J161" s="16" t="s">
+      <c r="J165" s="16" t="s">
         <v>699</v>
       </c>
-      <c r="K161" s="16" t="s">
+      <c r="K165" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="L161" s="16" t="s">
+      <c r="L165" s="16" t="s">
         <v>700</v>
       </c>
-      <c r="M161" s="17"/>
-    </row>
-    <row r="162" spans="1:13" ht="12.75">
-      <c r="A162" s="15" t="s">
+      <c r="M165" s="17"/>
+    </row>
+    <row r="166" spans="1:13" ht="12.75">
+      <c r="A166" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="B162" s="51" t="s">
+      <c r="B166" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="C162" s="16" t="s">
+      <c r="C166" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="D162" s="16" t="s">
+      <c r="D166" s="16" t="s">
         <v>2602</v>
       </c>
-      <c r="E162" s="16" t="s">
+      <c r="E166" s="16" t="s">
         <v>2603</v>
       </c>
-      <c r="F162" s="16"/>
-      <c r="G162" s="16"/>
-      <c r="H162" s="16"/>
-      <c r="I162" s="16" t="s">
+      <c r="F166" s="16"/>
+      <c r="G166" s="16"/>
+      <c r="H166" s="16"/>
+      <c r="I166" s="16" t="s">
         <v>2604</v>
       </c>
-      <c r="J162" s="16" t="s">
+      <c r="J166" s="16" t="s">
         <v>2310</v>
       </c>
-      <c r="K162" s="16" t="s">
+      <c r="K166" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="L162" s="16" t="s">
+      <c r="L166" s="16" t="s">
         <v>2607</v>
       </c>
-      <c r="M162" s="17"/>
-    </row>
-    <row r="163" spans="1:13" ht="12.75">
-      <c r="A163" s="15" t="s">
+      <c r="M166" s="17"/>
+    </row>
+    <row r="167" spans="1:13" ht="12.75">
+      <c r="A167" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="B163" s="51" t="s">
+      <c r="B167" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="C163" s="16" t="s">
+      <c r="C167" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="D163" s="16" t="s">
+      <c r="D167" s="16" t="s">
         <v>2602</v>
       </c>
-      <c r="E163" s="16" t="s">
+      <c r="E167" s="16" t="s">
         <v>2603</v>
       </c>
-      <c r="F163" s="16"/>
-      <c r="G163" s="16"/>
-      <c r="H163" s="16"/>
-      <c r="I163" s="16" t="s">
+      <c r="F167" s="16"/>
+      <c r="G167" s="16"/>
+      <c r="H167" s="16"/>
+      <c r="I167" s="16" t="s">
         <v>2604</v>
       </c>
-      <c r="J163" s="16" t="s">
+      <c r="J167" s="16" t="s">
         <v>2314</v>
       </c>
-      <c r="K163" s="16" t="s">
+      <c r="K167" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="L163" s="16" t="s">
+      <c r="L167" s="16" t="s">
         <v>2608</v>
       </c>
-      <c r="M163" s="17"/>
-    </row>
-    <row r="164" spans="1:13" ht="12.75">
-      <c r="A164" s="15" t="s">
+      <c r="M167" s="17"/>
+    </row>
+    <row r="168" spans="1:13" ht="12.75">
+      <c r="A168" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="B164" s="51" t="s">
+      <c r="B168" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="C164" s="16" t="s">
+      <c r="C168" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="D164" s="16" t="s">
+      <c r="D168" s="16" t="s">
         <v>2602</v>
       </c>
-      <c r="E164" s="16" t="s">
+      <c r="E168" s="16" t="s">
         <v>2603</v>
       </c>
-      <c r="F164" s="16"/>
-      <c r="G164" s="16"/>
-      <c r="H164" s="16"/>
-      <c r="I164" s="16" t="s">
+      <c r="F168" s="16"/>
+      <c r="G168" s="16"/>
+      <c r="H168" s="16"/>
+      <c r="I168" s="16" t="s">
         <v>2604</v>
       </c>
-      <c r="J164" s="16" t="s">
+      <c r="J168" s="16" t="s">
         <v>2605</v>
       </c>
-      <c r="K164" s="16" t="s">
+      <c r="K168" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="L164" s="16" t="s">
+      <c r="L168" s="16" t="s">
         <v>2609</v>
       </c>
-      <c r="M164" s="17"/>
-    </row>
-    <row r="165" spans="1:13" ht="12.75">
-      <c r="A165" s="7" t="s">
+      <c r="M168" s="17"/>
+    </row>
+    <row r="169" spans="1:13" ht="12.75">
+      <c r="A169" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="B165" s="14" t="s">
+      <c r="B169" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C169" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="D165" s="8" t="s">
+      <c r="D169" s="8" t="s">
         <v>2602</v>
       </c>
-      <c r="E165" s="8" t="s">
+      <c r="E169" s="8" t="s">
         <v>2603</v>
       </c>
-      <c r="F165" s="8"/>
-      <c r="G165" s="8"/>
-      <c r="H165" s="8"/>
-      <c r="I165" s="8" t="s">
+      <c r="F169" s="8"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="8"/>
+      <c r="I169" s="8" t="s">
         <v>2604</v>
       </c>
-      <c r="J165" s="8" t="s">
+      <c r="J169" s="8" t="s">
         <v>2606</v>
       </c>
-      <c r="K165" s="8" t="s">
+      <c r="K169" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="L165" s="8" t="s">
+      <c r="L169" s="8" t="s">
         <v>2610</v>
       </c>
-      <c r="M165" s="10"/>
+      <c r="M169" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -43811,9 +43972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>

<commit_message>
Atualização Documentação Controle Tabelas NOVA
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Sequência Execução" sheetId="35" r:id="rId1"/>
@@ -9360,8 +9360,8 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -9889,10 +9889,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -15456,7 +15456,7 @@
     <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23:I23"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -17123,10 +17123,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -19622,8 +19622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A8"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -30296,8 +30296,8 @@
   <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -38384,7 +38384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I123" sqref="I123"/>
     </sheetView>
@@ -43972,9 +43972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>

<commit_message>
Documentação Controle Tabelas NOVA
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="27" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="Sequência Execução" sheetId="35" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11122" uniqueCount="3058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11140" uniqueCount="3069">
   <si>
     <t>Processo de Carga LN</t>
   </si>
@@ -9221,6 +9221,39 @@
   </si>
   <si>
     <t>ln.ods_wms_tracking_pedido</t>
+  </si>
+  <si>
+    <t>CAR_Cliente_B2B</t>
+  </si>
+  <si>
+    <t>N:\Migracao\CAR_Cliente_B2B\ssis_controlador_car_cliente_b2b.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) Controlador CAR Cliente B2B</t>
+  </si>
+  <si>
+    <t>N:\Migracao\CAR_Cliente_B2B\stg_car_cliente_b2b.dtsx</t>
+  </si>
+  <si>
+    <t>N:\Migracao\CAR_Cliente_B2B\ods_car_cliente_b2b.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) Carrega STG</t>
+  </si>
+  <si>
+    <t>(DFT) STG CAR Cliente B2B</t>
+  </si>
+  <si>
+    <t>dbo.stg_car_cliente_b2b</t>
+  </si>
+  <si>
+    <t>(SC) Carrega ODS</t>
+  </si>
+  <si>
+    <t>(DFT) ODS Cliente B2B</t>
+  </si>
+  <si>
+    <t>ln.ods_car_cliente_b2b</t>
   </si>
 </sst>
 </file>
@@ -30942,7 +30975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
@@ -37372,10 +37405,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="A127" sqref="A127"/>
+      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -40646,27 +40679,63 @@
       <c r="J126" s="17"/>
     </row>
     <row r="127" spans="1:10">
-      <c r="A127" s="48"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="16"/>
-      <c r="D127" s="16"/>
-      <c r="E127" s="16"/>
-      <c r="F127" s="16"/>
-      <c r="G127" s="16"/>
-      <c r="H127" s="49"/>
-      <c r="I127" s="49"/>
+      <c r="A127" s="48" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>3059</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>3060</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="E127" s="16" t="s">
+        <v>3061</v>
+      </c>
+      <c r="F127" s="16" t="s">
+        <v>3063</v>
+      </c>
+      <c r="G127" s="16" t="s">
+        <v>3064</v>
+      </c>
+      <c r="H127" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="I127" s="49" t="s">
+        <v>3065</v>
+      </c>
       <c r="J127" s="17"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="48"/>
-      <c r="B128" s="16"/>
-      <c r="C128" s="16"/>
-      <c r="D128" s="16"/>
-      <c r="E128" s="16"/>
-      <c r="F128" s="16"/>
-      <c r="G128" s="16"/>
-      <c r="H128" s="49"/>
-      <c r="I128" s="49"/>
+      <c r="A128" s="48" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>3059</v>
+      </c>
+      <c r="C128" s="16" t="s">
+        <v>3060</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="E128" s="16" t="s">
+        <v>3062</v>
+      </c>
+      <c r="F128" s="16" t="s">
+        <v>3066</v>
+      </c>
+      <c r="G128" s="16" t="s">
+        <v>3067</v>
+      </c>
+      <c r="H128" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="I128" s="49" t="s">
+        <v>3068</v>
+      </c>
       <c r="J128" s="17"/>
     </row>
     <row r="129" spans="1:10">

</xml_diff>

<commit_message>
Atualização Controle de Tabelas - CNOVA
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NOVA-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="27" activeTab="33"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sequência Execução" sheetId="35" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11140" uniqueCount="3069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11146" uniqueCount="3071">
   <si>
     <t>Processo de Carga LN</t>
   </si>
@@ -9254,6 +9254,12 @@
   </si>
   <si>
     <t>ln.ods_car_cliente_b2b</t>
+  </si>
+  <si>
+    <t>(DFT) Trp - Transporte</t>
+  </si>
+  <si>
+    <t>ln.ods_trp_transporte</t>
   </si>
 </sst>
 </file>
@@ -30973,11 +30979,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J130"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -34556,22 +34562,22 @@
         <v>0</v>
       </c>
       <c r="B125" s="42" t="s">
-        <v>282</v>
+        <v>393</v>
       </c>
       <c r="C125" s="42"/>
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
       <c r="F125" s="42" t="s">
-        <v>264</v>
+        <v>3053</v>
       </c>
       <c r="G125" s="42" t="s">
-        <v>265</v>
+        <v>3069</v>
       </c>
       <c r="H125" s="42" t="s">
         <v>213</v>
       </c>
       <c r="I125" s="42" t="s">
-        <v>266</v>
+        <v>3070</v>
       </c>
       <c r="J125" s="43"/>
     </row>
@@ -34589,13 +34595,13 @@
         <v>264</v>
       </c>
       <c r="G126" s="42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H126" s="42" t="s">
         <v>213</v>
       </c>
       <c r="I126" s="42" t="s">
-        <v>2591</v>
+        <v>266</v>
       </c>
       <c r="J126" s="43"/>
     </row>
@@ -34613,13 +34619,13 @@
         <v>264</v>
       </c>
       <c r="G127" s="42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H127" s="42" t="s">
         <v>213</v>
       </c>
       <c r="I127" s="42" t="s">
-        <v>269</v>
+        <v>2591</v>
       </c>
       <c r="J127" s="43"/>
     </row>
@@ -34637,13 +34643,13 @@
         <v>264</v>
       </c>
       <c r="G128" s="42" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H128" s="42" t="s">
         <v>213</v>
       </c>
       <c r="I128" s="42" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J128" s="43"/>
     </row>
@@ -34658,44 +34664,68 @@
       <c r="D129" s="42"/>
       <c r="E129" s="42"/>
       <c r="F129" s="42" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G129" s="42" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H129" s="42" t="s">
         <v>213</v>
       </c>
       <c r="I129" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="J129" s="43"/>
+    </row>
+    <row r="130" spans="1:10" s="44" customFormat="1">
+      <c r="A130" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="C130" s="42"/>
+      <c r="D130" s="42"/>
+      <c r="E130" s="42"/>
+      <c r="F130" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="G130" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="H130" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="I130" s="42" t="s">
         <v>274</v>
       </c>
-      <c r="J129" s="43" t="s">
+      <c r="J130" s="43" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
-      <c r="A130" s="7" t="s">
+    <row r="131" spans="1:10">
+      <c r="A131" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B131" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8" t="s">
+      <c r="C131" s="8"/>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8"/>
+      <c r="F131" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="G130" s="8" t="s">
+      <c r="G131" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="H130" s="8" t="s">
+      <c r="H131" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="I130" s="8" t="s">
+      <c r="I131" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="J130" s="10"/>
+      <c r="J131" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -37405,10 +37435,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>